<commit_message>
re-arrange and add missing images
</commit_message>
<xml_diff>
--- a/fujimi-gamebook/checklist.xlsx
+++ b/fujimi-gamebook/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/fujimi-gamebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333D64F5-A55B-C247-B349-54E52243A74A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3274353-0D3D-8B41-B519-4B41DCDA0618}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{28801664-8CDC-BD45-BDED-0E88B39C2FBF}"/>
   </bookViews>
@@ -318,9 +318,6 @@
     <t>Moonshae Saga 4: The Prophecy of the Dead Queen</t>
   </si>
   <si>
-    <t>moonshae4.jpeg</t>
-  </si>
-  <si>
     <t>3-4</t>
   </si>
   <si>
@@ -469,6 +466,9 @@
   </si>
   <si>
     <t>9-4</t>
+  </si>
+  <si>
+    <t>moonshae4.jpg</t>
   </si>
 </sst>
 </file>
@@ -833,10 +833,13 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -1222,48 +1225,48 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1271,22 +1274,22 @@
         <v>1989</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1294,160 +1297,160 @@
         <v>1989</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="F21" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>144</v>
       </c>
       <c r="F25" t="s">
         <v>10</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1455,22 +1458,22 @@
         <v>1986</v>
       </c>
       <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
         <v>104</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
         <v>105</v>
       </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="F28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1478,22 +1481,22 @@
         <v>1986</v>
       </c>
       <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" t="s">
         <v>108</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
         <v>109</v>
       </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="F29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1501,22 +1504,22 @@
         <v>1986</v>
       </c>
       <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" t="s">
         <v>112</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
         <v>113</v>
       </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="F30" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1524,22 +1527,22 @@
         <v>1987</v>
       </c>
       <c r="B31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" t="s">
         <v>116</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
         <v>117</v>
       </c>
-      <c r="D31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1547,16 +1550,16 @@
         <v>1987</v>
       </c>
       <c r="B32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" t="s">
         <v>120</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
         <v>121</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" t="s">
-        <v>122</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
@@ -1568,16 +1571,16 @@
         <v>1989</v>
       </c>
       <c r="B33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
         <v>123</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
         <v>124</v>
-      </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" t="s">
-        <v>125</v>
       </c>
       <c r="F33" t="s">
         <v>73</v>
@@ -1591,16 +1594,16 @@
         <v>1991</v>
       </c>
       <c r="B34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
         <v>126</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
         <v>127</v>
-      </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" t="s">
-        <v>128</v>
       </c>
       <c r="F34" t="s">
         <v>10</v>
@@ -1612,22 +1615,22 @@
         <v>1986</v>
       </c>
       <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" t="s">
         <v>129</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
         <v>130</v>
       </c>
-      <c r="D35" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="F35" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1635,22 +1638,22 @@
         <v>1986</v>
       </c>
       <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" t="s">
         <v>133</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
         <v>134</v>
       </c>
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="F36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1658,22 +1661,22 @@
         <v>1986</v>
       </c>
       <c r="B37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" t="s">
         <v>137</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
         <v>138</v>
       </c>
-      <c r="D37" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="F37" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1681,22 +1684,22 @@
         <v>1987</v>
       </c>
       <c r="B38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" t="s">
         <v>141</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
         <v>142</v>
       </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="F38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>